<commit_message>
files used for IRP comparison
</commit_message>
<xml_diff>
--- a/suppxls/Scen_ELC_IRP_Forced2030.xlsx
+++ b/suppxls/Scen_ELC_IRP_Forced2030.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\suppxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93838331-9D78-4EC6-9436-7E2E02C57038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A0A7AB2-5FB4-4D42-81D8-96C32E48AD1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4500" yWindow="-16605" windowWidth="23835" windowHeight="15255" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Define REFIT" sheetId="2" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="92">
   <si>
     <t>PSET_PN</t>
   </si>
@@ -274,6 +274,87 @@
   </si>
   <si>
     <t>hydro project</t>
+  </si>
+  <si>
+    <t>UC_N</t>
+  </si>
+  <si>
+    <t>UC_ATTR</t>
+  </si>
+  <si>
+    <t>Pset_PN</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>UC_NCAP</t>
+  </si>
+  <si>
+    <t>UC_NCAP~RHS</t>
+  </si>
+  <si>
+    <t>UC_RHSRT~0</t>
+  </si>
+  <si>
+    <t>UC_Growth_Wind</t>
+  </si>
+  <si>
+    <t>NCAP,GROWTH</t>
+  </si>
+  <si>
+    <t>ERW*</t>
+  </si>
+  <si>
+    <t>LO</t>
+  </si>
+  <si>
+    <t>UC_Growth_PV</t>
+  </si>
+  <si>
+    <t>ERSOLP*</t>
+  </si>
+  <si>
+    <t>UC_Growth_Batteries</t>
+  </si>
+  <si>
+    <t>~TFM_INS</t>
+  </si>
+  <si>
+    <t>REGION1</t>
+  </si>
+  <si>
+    <t>NCAP_START</t>
+  </si>
+  <si>
+    <t>ULGTGRLFSRU-N</t>
+  </si>
+  <si>
+    <t>IMPGRL</t>
+  </si>
+  <si>
+    <t>UC_RHSRT</t>
+  </si>
+  <si>
+    <t>UC_Sets: R_E: REGION1</t>
+  </si>
+  <si>
+    <t>UC_Sets: T_E:</t>
+  </si>
+  <si>
+    <t>UC_T</t>
+  </si>
+  <si>
+    <t>Bruno: I can't seem to get this to work so creating a new UC_ELC-IRP.</t>
+  </si>
+  <si>
+    <t>CSET_CN</t>
+  </si>
+  <si>
+    <t>ELCC</t>
+  </si>
+  <si>
+    <t>COM_PKRSV</t>
   </si>
 </sst>
 </file>
@@ -284,7 +365,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="[$£-809]#,##0.000;[Red]&quot;-&quot;[$£-809]#,##0.000"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -414,8 +495,27 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -449,8 +549,32 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="51"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -470,6 +594,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -580,13 +713,29 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="98">
     <cellStyle name="20% - Accent5 2" xfId="44" xr:uid="{2E09701F-C8AC-44F3-9A2D-DF9315D4D18B}"/>
@@ -1065,19 +1214,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:Q54"/>
+  <dimension ref="B2:Q66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4:L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
     <col min="4" max="6" width="13.85546875" customWidth="1"/>
     <col min="7" max="7" width="13.5703125" customWidth="1"/>
     <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" customWidth="1"/>
     <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="8.42578125" bestFit="1" customWidth="1"/>
@@ -1149,11 +1299,21 @@
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
+      <c r="H4" s="3">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0</v>
+      </c>
+      <c r="L4" s="3">
+        <v>0</v>
+      </c>
       <c r="M4" s="3"/>
       <c r="N4" s="3" t="s">
         <v>61</v>
@@ -1174,11 +1334,21 @@
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
+      <c r="H5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0</v>
+      </c>
+      <c r="L5" s="3">
+        <v>0</v>
+      </c>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
     </row>
@@ -1554,37 +1724,37 @@
       <c r="N15" s="3"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E16" t="s">
-        <v>5</v>
-      </c>
-      <c r="F16" s="3">
-        <v>0</v>
-      </c>
-      <c r="G16" s="3">
+      <c r="E16" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="14">
+        <v>0</v>
+      </c>
+      <c r="G16" s="14">
         <v>0.64400000000000002</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H16" s="14">
         <v>0.14000000000000001</v>
       </c>
-      <c r="I16" s="3">
+      <c r="I16" s="14">
         <v>0.68400000000000005</v>
       </c>
-      <c r="J16" s="3">
-        <v>0</v>
-      </c>
-      <c r="K16" s="3">
+      <c r="J16" s="14">
+        <v>0</v>
+      </c>
+      <c r="K16" s="14">
         <v>1.5</v>
       </c>
-      <c r="L16" s="3">
+      <c r="L16" s="14">
         <v>1.5</v>
       </c>
       <c r="N16" s="3"/>
@@ -1890,37 +2060,37 @@
       <c r="N24" s="3"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E25" t="s">
-        <v>5</v>
-      </c>
-      <c r="F25" s="3">
-        <v>0</v>
-      </c>
-      <c r="G25" s="3">
+      <c r="E25" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" s="14">
+        <v>0</v>
+      </c>
+      <c r="G25" s="14">
         <v>0.51300000000000001</v>
       </c>
-      <c r="H25" s="3">
-        <v>0</v>
-      </c>
-      <c r="I25" s="3">
+      <c r="H25" s="14">
+        <v>0</v>
+      </c>
+      <c r="I25" s="14">
         <v>2.6150000000000002</v>
       </c>
-      <c r="J25" s="3">
+      <c r="J25" s="14">
         <v>0.61499999999999999</v>
       </c>
-      <c r="K25" s="3">
-        <v>0</v>
-      </c>
-      <c r="L25" s="3">
+      <c r="K25" s="14">
+        <v>0</v>
+      </c>
+      <c r="L25" s="14">
         <f>L18</f>
         <v>0.68799999999999994</v>
       </c>
@@ -2180,7 +2350,7 @@
       <c r="M32" s="3"/>
       <c r="N32" s="3"/>
     </row>
-    <row r="33" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F33" s="3">
         <v>0.2678571428571429</v>
       </c>
@@ -2193,41 +2363,622 @@
       <c r="M33" s="3"/>
       <c r="N33" s="3"/>
     </row>
-    <row r="34" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F34">
         <v>9.7500000000000003E-2</v>
       </c>
     </row>
-    <row r="35" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F35">
         <v>0.19500000000000001</v>
       </c>
     </row>
-    <row r="36" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F36">
         <v>0.7242857142857142</v>
       </c>
     </row>
-    <row r="37" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F37">
         <v>0.21535714285714302</v>
       </c>
     </row>
-    <row r="52" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-    </row>
-    <row r="53" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
-      <c r="G53" s="2"/>
-    </row>
-    <row r="54" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C54" s="3"/>
+    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C40" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D40" s="1"/>
+      <c r="H40" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I40" s="1"/>
+    </row>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C41" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E41" t="s">
+        <v>80</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J41">
+        <v>2025</v>
+      </c>
+      <c r="K41">
+        <v>2028</v>
+      </c>
+      <c r="L41">
+        <v>2030</v>
+      </c>
+      <c r="M41">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>82</v>
+      </c>
+      <c r="D42" t="s">
+        <v>81</v>
+      </c>
+      <c r="E42">
+        <v>2025</v>
+      </c>
+      <c r="H42" t="s">
+        <v>90</v>
+      </c>
+      <c r="I42" t="s">
+        <v>91</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+      <c r="K42">
+        <v>0</v>
+      </c>
+      <c r="L42">
+        <v>0</v>
+      </c>
+      <c r="M42">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>83</v>
+      </c>
+      <c r="D43" t="s">
+        <v>81</v>
+      </c>
+      <c r="E43">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B47" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D47" s="5"/>
+    </row>
+    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B48" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D48" s="5"/>
+      <c r="E48" s="6"/>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G49" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B50" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F50" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G50" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H50" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="I50" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="J50" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B51" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E51">
+        <v>2025</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G51">
+        <v>100</v>
+      </c>
+      <c r="H51">
+        <v>1</v>
+      </c>
+      <c r="I51">
+        <v>-1.5</v>
+      </c>
+      <c r="J51" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B52" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E52">
+        <v>2026</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G52">
+        <v>100</v>
+      </c>
+      <c r="H52">
+        <v>1</v>
+      </c>
+      <c r="I52">
+        <v>-1.5</v>
+      </c>
+      <c r="J52" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B53" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E53">
+        <v>2030</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G53">
+        <v>100</v>
+      </c>
+      <c r="H53">
+        <v>1</v>
+      </c>
+      <c r="I53">
+        <v>-1.5</v>
+      </c>
+      <c r="J53" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B54" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E54">
+        <v>2031</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G54">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B55" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E55">
+        <v>2054</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G55">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H55">
+        <v>1</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B56" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E56">
+        <v>2055</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G56">
+        <v>100</v>
+      </c>
+      <c r="H56">
+        <v>1</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+      <c r="J56" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B57" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E57">
+        <v>2026</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G57">
+        <v>100</v>
+      </c>
+      <c r="H57">
+        <v>1</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
+      </c>
+      <c r="J57" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B58" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E58">
+        <f>E53</f>
+        <v>2030</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G58">
+        <v>100</v>
+      </c>
+      <c r="H58">
+        <v>1</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+      <c r="J58" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B59" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E59">
+        <f>E54</f>
+        <v>2031</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G59">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H59">
+        <v>1</v>
+      </c>
+      <c r="I59">
+        <v>0</v>
+      </c>
+      <c r="J59" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B60" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E60">
+        <v>2054</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G60">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H60">
+        <v>1</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+      <c r="J60" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B61" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E61">
+        <v>2055</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G61">
+        <v>100</v>
+      </c>
+      <c r="H61">
+        <v>1</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B62" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E62">
+        <v>2026</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G62">
+        <v>100</v>
+      </c>
+      <c r="H62">
+        <v>1</v>
+      </c>
+      <c r="I62">
+        <v>-2.7</v>
+      </c>
+      <c r="J62" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B63" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E63">
+        <v>2030</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G63">
+        <v>100</v>
+      </c>
+      <c r="H63">
+        <v>1</v>
+      </c>
+      <c r="I63">
+        <v>-2.7</v>
+      </c>
+      <c r="J63" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B64" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E64">
+        <v>2031</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G64">
+        <v>1.5</v>
+      </c>
+      <c r="H64">
+        <v>1</v>
+      </c>
+      <c r="I64">
+        <v>0</v>
+      </c>
+      <c r="J64" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B65" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E65">
+        <v>2054</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G65">
+        <v>1.5</v>
+      </c>
+      <c r="H65">
+        <v>1</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
+      </c>
+      <c r="J65" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B66" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E66">
+        <v>2055</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G66">
+        <v>100</v>
+      </c>
+      <c r="H66">
+        <v>1</v>
+      </c>
+      <c r="I66">
+        <v>0</v>
+      </c>
+      <c r="J66" s="5">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
With IRP updates (note that IPP changes from earlier commit is here)
</commit_message>
<xml_diff>
--- a/suppxls/Scen_ELC_IRP_Forced2030.xlsx
+++ b/suppxls/Scen_ELC_IRP_Forced2030.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\suppxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A0A7AB2-5FB4-4D42-81D8-96C32E48AD1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{270A7B9D-982F-4E74-8D05-1E1EE7B7C2ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4500" yWindow="-16605" windowWidth="23835" windowHeight="15255" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2430" yWindow="150" windowWidth="24630" windowHeight="15330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Define REFIT" sheetId="2" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <definedNames>
     <definedName name="_AtRisk_SimSetting_AutomaticallyGenerateReports" hidden="1">FALSE</definedName>
     <definedName name="_AtRisk_SimSetting_AutomaticResultsDisplayMode" hidden="1">0</definedName>
@@ -78,8 +81,98 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={DFB42807-3B81-4EC4-B1B8-E2021C8A0185}</author>
+    <author>tc={CE2E4170-1CA7-4B5E-981F-45C13735EC1B}</author>
+    <author>tc={45EF0A99-A55A-49FF-919A-FB3C79A72DD0}</author>
+    <author>tc={37514907-33CA-4750-A216-B58357461AC2}</author>
+    <author>tc={1C09159B-FFF8-49C5-8CA1-6B577EF67A54}</author>
+    <author>tc={7F15C7F4-8D8F-4675-AACC-580495CB6716}</author>
+    <author>tc={996E6D14-20D9-40B3-88A7-1B70E029103F}</author>
+    <author>tc={AE79E564-FDAC-41E4-866B-DBB281531206}</author>
+    <author>tc={F856E498-309C-4C3A-9A1F-40A076B2729A}</author>
+  </authors>
+  <commentList>
+    <comment ref="F15" authorId="0" shapeId="0" xr:uid="{DFB42807-3B81-4EC4-B1B8-E2021C8A0185}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    0.330 is part of the Scatec hybrid plant</t>
+      </text>
+    </comment>
+    <comment ref="G15" authorId="1" shapeId="0" xr:uid="{CE2E4170-1CA7-4B5E-981F-45C13735EC1B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Extras from RMIPPP hybrid plants</t>
+      </text>
+    </comment>
+    <comment ref="H15" authorId="2" shapeId="0" xr:uid="{45EF0A99-A55A-49FF-919A-FB3C79A72DD0}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Missing Acwa hybrid plant added here</t>
+      </text>
+    </comment>
+    <comment ref="R15" authorId="3" shapeId="0" xr:uid="{37514907-33CA-4750-A216-B58357461AC2}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Error because RMIPPP and "Dispatchable" included here.</t>
+      </text>
+    </comment>
+    <comment ref="G16" authorId="4" shapeId="0" xr:uid="{1C09159B-FFF8-49C5-8CA1-6B577EF67A54}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Extras taken from estimates for hybrid plants from RMIPPP</t>
+      </text>
+    </comment>
+    <comment ref="R16" authorId="5" shapeId="0" xr:uid="{7F15C7F4-8D8F-4675-AACC-580495CB6716}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Error because of RMIPPP</t>
+      </text>
+    </comment>
+    <comment ref="F25" authorId="6" shapeId="0" xr:uid="{996E6D14-20D9-40B3-88A7-1B70E029103F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Including Scatec hybrid plant</t>
+      </text>
+    </comment>
+    <comment ref="H25" authorId="7" shapeId="0" xr:uid="{AE79E564-FDAC-41E4-866B-DBB281531206}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Missing Acwa hybrid plant added here</t>
+      </text>
+    </comment>
+    <comment ref="R25" authorId="8" shapeId="0" xr:uid="{F856E498-309C-4C3A-9A1F-40A076B2729A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Error because RMIPPP and "Dispatchable" included here.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="130">
   <si>
     <t>PSET_PN</t>
   </si>
@@ -355,15 +448,132 @@
   </si>
   <si>
     <t>COM_PKRSV</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>From slide</t>
+  </si>
+  <si>
+    <t>error</t>
+  </si>
+  <si>
+    <t>Figure 8 is not used in Reference</t>
+  </si>
+  <si>
+    <t>Using info from slide, and not Table 2.</t>
+  </si>
+  <si>
+    <t>Assumed Tech split</t>
+  </si>
+  <si>
+    <t>Assumed CF</t>
+  </si>
+  <si>
+    <t>Share of energy</t>
+  </si>
+  <si>
+    <t>Energy (GWh)</t>
+  </si>
+  <si>
+    <t>Project Name</t>
+  </si>
+  <si>
+    <t>Price R/MWh</t>
+  </si>
+  <si>
+    <t>Capacity (MW)</t>
+  </si>
+  <si>
+    <t>Solar</t>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>Storage</t>
+  </si>
+  <si>
+    <t>Overall CF</t>
+  </si>
+  <si>
+    <t>GWh</t>
+  </si>
+  <si>
+    <t>Storage Losses</t>
+  </si>
+  <si>
+    <t>Oya_Energy_Hybrid_Facility</t>
+  </si>
+  <si>
+    <t>ACWA_Power_Project_DAO</t>
+  </si>
+  <si>
+    <t>Umoyilanga_Energy</t>
+  </si>
+  <si>
+    <t>Karpowership_SA_Coega</t>
+  </si>
+  <si>
+    <t>Karpowership_SA_Richards_Bay</t>
+  </si>
+  <si>
+    <t>Karpowership_SA_Saldanha</t>
+  </si>
+  <si>
+    <t>Mulilo_Total_Coega</t>
+  </si>
+  <si>
+    <t>Mulilo_Total_Hydra_Storage</t>
+  </si>
+  <si>
+    <t>Total Firm</t>
+  </si>
+  <si>
+    <t>https://www.ipp-rm.co.za/</t>
+  </si>
+  <si>
+    <t>due in 2026 according to: https://www.acwapower.com/news/acwa-power-signs-power-purchase-agreement-for-south-africas-largest-hybrid-dispatchable-renewable-energy-project/</t>
+  </si>
+  <si>
+    <t>missing</t>
+  </si>
+  <si>
+    <t>financial close by August 2022, online by 2024</t>
+  </si>
+  <si>
+    <t>MW solar</t>
+  </si>
+  <si>
+    <t>MW</t>
+  </si>
+  <si>
+    <t>batteries</t>
+  </si>
+  <si>
+    <t>MWH</t>
+  </si>
+  <si>
+    <t>Scatec</t>
+  </si>
+  <si>
+    <t>hours</t>
+  </si>
+  <si>
+    <t>Total Excluding KarPower</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="2">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="[$£-809]#,##0.000;[Red]&quot;-&quot;[$£-809]#,##0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="0.0000"/>
   </numFmts>
   <fonts count="23" x14ac:knownFonts="1">
     <font>
@@ -713,7 +923,7 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
@@ -736,6 +946,14 @@
     <xf numFmtId="0" fontId="22" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="4" fillId="9" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="17" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="4" fillId="9" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="98">
     <cellStyle name="20% - Accent5 2" xfId="44" xr:uid="{2E09701F-C8AC-44F3-9A2D-DF9315D4D18B}"/>
@@ -882,16 +1100,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>94553</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>77257</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9886</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>541574</xdr:colOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>33574</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>84849</xdr:rowOff>
+      <xdr:rowOff>182</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -914,8 +1132,228 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10934700" y="94553"/>
-          <a:ext cx="8504474" cy="5514796"/>
+          <a:off x="15084424" y="200386"/>
+          <a:ext cx="8549983" cy="5514796"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>599401</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>52916</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>213365</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>84667</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4AA9C4C-9BB0-3F27-8610-760A875E510F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="25912089" y="1005416"/>
+          <a:ext cx="6900589" cy="4413251"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>238126</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>564863</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>94548</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA62E07C-F795-5607-3B8D-5925895A18BD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15228095" y="5715000"/>
+          <a:ext cx="10649456" cy="5619048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>337024</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>74472</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78DA12E6-F7F9-4006-8462-549C18CE6CEF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13870781" y="15068550"/>
+          <a:ext cx="8742837" cy="4627422"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>7143</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>184673</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>36135</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF1F4E15-BC6A-4822-818F-14C6F29B0A7B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22890956" y="15049500"/>
+          <a:ext cx="6856936" cy="4989135"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>251618</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>42312</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65DA6BAA-32D6-468D-AD13-593964B3D707}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13870781" y="20193000"/>
+          <a:ext cx="6835775" cy="2328312"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -925,6 +1363,136 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Index"/>
+      <sheetName val="Assumptions"/>
+      <sheetName val="Processes"/>
+      <sheetName val="Commodities"/>
+      <sheetName val="tables for reports"/>
+      <sheetName val="ProcDataGenPre2012"/>
+      <sheetName val="ProcDataGen2012On"/>
+      <sheetName val="ProcDataRECostProfiles"/>
+      <sheetName val="ProcDataTnD"/>
+      <sheetName val="ProcDataExports"/>
+      <sheetName val="ProcDataMines"/>
+      <sheetName val="CommData"/>
+      <sheetName val="ProcDataRM"/>
+      <sheetName val="ProcDataAux"/>
+      <sheetName val="ProcDataLowEAF"/>
+      <sheetName val="ProcDataEndoRetire"/>
+      <sheetName val="ProcDataRampRates"/>
+      <sheetName val="JETPsep22"/>
+      <sheetName val="EskomCoalPrice2019"/>
+      <sheetName val="eskom production 2009-YTD"/>
+      <sheetName val="eskom fuel 2009-YTD"/>
+      <sheetName val="HistoricalDispatch"/>
+      <sheetName val="DecomSchedule"/>
+      <sheetName val="NERSA2017"/>
+      <sheetName val="NERSA2018"/>
+      <sheetName val="EskomCoalNERSACombined"/>
+      <sheetName val="RMIPPPP"/>
+      <sheetName val="REIPPP"/>
+      <sheetName val="OnsitePV"/>
+      <sheetName val="IRP Costs"/>
+      <sheetName val="PumpStorage"/>
+      <sheetName val="NBI_NREL_etc"/>
+      <sheetName val="CoalIPP"/>
+      <sheetName val="FGD costs"/>
+      <sheetName val="PWR_Lab"/>
+      <sheetName val="Lab.Calcs.Assumptions"/>
+      <sheetName val="SAM"/>
+      <sheetName val="SAM2019"/>
+      <sheetName val="From SAM"/>
+      <sheetName val="ElecBY"/>
+      <sheetName val="Deflator"/>
+      <sheetName val="ANSv2-692-REGIONS"/>
+      <sheetName val="ANSv2-692-Commodities"/>
+      <sheetName val="ANSv2-692-Processes"/>
+      <sheetName val="ANSv2-692-Constraints"/>
+      <sheetName val="ANSv2-692-CommData"/>
+      <sheetName val="ANSv2-692-ProcData"/>
+      <sheetName val="ANSv2-692-ConstrData"/>
+      <sheetName val="ANSv2-692-ITEMS"/>
+      <sheetName val="ANSv2-692-TS DATA"/>
+      <sheetName val="ANSv2-692-TID DATA"/>
+      <sheetName val="ANSv2-692-TS&amp;TID DATA"/>
+      <sheetName val="ANSv2-692-TS TRADE"/>
+      <sheetName val="ANSv2-692-TID TRADE"/>
+      <sheetName val="ANSv2-692-TS&amp;TID TRADE"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
+      <sheetData sheetId="30"/>
+      <sheetData sheetId="31"/>
+      <sheetData sheetId="32"/>
+      <sheetData sheetId="33"/>
+      <sheetData sheetId="34"/>
+      <sheetData sheetId="35"/>
+      <sheetData sheetId="36"/>
+      <sheetData sheetId="37"/>
+      <sheetData sheetId="38"/>
+      <sheetData sheetId="39"/>
+      <sheetData sheetId="40"/>
+      <sheetData sheetId="41"/>
+      <sheetData sheetId="42"/>
+      <sheetData sheetId="43"/>
+      <sheetData sheetId="44"/>
+      <sheetData sheetId="45"/>
+      <sheetData sheetId="46"/>
+      <sheetData sheetId="47"/>
+      <sheetData sheetId="48"/>
+      <sheetData sheetId="49"/>
+      <sheetData sheetId="50"/>
+      <sheetData sheetId="51"/>
+      <sheetData sheetId="52"/>
+      <sheetData sheetId="53"/>
+      <sheetData sheetId="54"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Bruno Merven" id="{F5BA0DE9-979C-48B6-95A3-E4B0CF119240}" userId="S::01405439@wf.uct.ac.za::c7f06137-2c3b-4c5c-8f38-fe1abbc96860" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1212,12 +1780,44 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="F15" dT="2024-02-06T11:55:39.35" personId="{F5BA0DE9-979C-48B6-95A3-E4B0CF119240}" id="{DFB42807-3B81-4EC4-B1B8-E2021C8A0185}">
+    <text>0.330 is part of the Scatec hybrid plant</text>
+  </threadedComment>
+  <threadedComment ref="G15" dT="2024-02-06T12:01:20.26" personId="{F5BA0DE9-979C-48B6-95A3-E4B0CF119240}" id="{CE2E4170-1CA7-4B5E-981F-45C13735EC1B}">
+    <text>Extras from RMIPPP hybrid plants</text>
+  </threadedComment>
+  <threadedComment ref="H15" dT="2024-02-06T12:17:01.60" personId="{F5BA0DE9-979C-48B6-95A3-E4B0CF119240}" id="{45EF0A99-A55A-49FF-919A-FB3C79A72DD0}">
+    <text>Missing Acwa hybrid plant added here</text>
+  </threadedComment>
+  <threadedComment ref="R15" dT="2024-02-06T12:17:53.34" personId="{F5BA0DE9-979C-48B6-95A3-E4B0CF119240}" id="{37514907-33CA-4750-A216-B58357461AC2}">
+    <text>Error because RMIPPP and "Dispatchable" included here.</text>
+  </threadedComment>
+  <threadedComment ref="G16" dT="2024-02-06T11:58:37.91" personId="{F5BA0DE9-979C-48B6-95A3-E4B0CF119240}" id="{1C09159B-FFF8-49C5-8CA1-6B577EF67A54}">
+    <text>Extras taken from estimates for hybrid plants from RMIPPP</text>
+  </threadedComment>
+  <threadedComment ref="R16" dT="2024-02-06T12:18:06.05" personId="{F5BA0DE9-979C-48B6-95A3-E4B0CF119240}" id="{7F15C7F4-8D8F-4675-AACC-580495CB6716}">
+    <text>Error because of RMIPPP</text>
+  </threadedComment>
+  <threadedComment ref="F25" dT="2024-02-06T11:56:07.28" personId="{F5BA0DE9-979C-48B6-95A3-E4B0CF119240}" id="{996E6D14-20D9-40B3-88A7-1B70E029103F}">
+    <text>Including Scatec hybrid plant</text>
+  </threadedComment>
+  <threadedComment ref="H25" dT="2024-02-06T12:17:16.08" personId="{F5BA0DE9-979C-48B6-95A3-E4B0CF119240}" id="{AE79E564-FDAC-41E4-866B-DBB281531206}">
+    <text>Missing Acwa hybrid plant added here</text>
+  </threadedComment>
+  <threadedComment ref="R25" dT="2024-02-06T12:18:20.87" personId="{F5BA0DE9-979C-48B6-95A3-E4B0CF119240}" id="{F856E498-309C-4C3A-9A1F-40A076B2729A}">
+    <text>Error because RMIPPP and "Dispatchable" included here.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:Q66"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:AK123"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:L5"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="S75" sqref="S75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1237,7 +1837,12 @@
     <col min="17" max="18" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="2:37" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1246,7 +1851,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:37" ht="30" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1281,10 +1886,18 @@
       <c r="N3" s="2" t="s">
         <v>60</v>
       </c>
+      <c r="O3" t="s">
+        <v>92</v>
+      </c>
       <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q3" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
@@ -1318,8 +1931,11 @@
       <c r="N4" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="AK4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
@@ -1352,7 +1968,7 @@
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
@@ -1389,7 +2005,7 @@
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
@@ -1426,7 +2042,7 @@
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>16</v>
       </c>
@@ -1463,7 +2079,7 @@
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
@@ -1500,7 +2116,7 @@
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>20</v>
       </c>
@@ -1537,7 +2153,7 @@
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>22</v>
       </c>
@@ -1574,7 +2190,7 @@
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>24</v>
       </c>
@@ -1611,7 +2227,7 @@
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
@@ -1648,7 +2264,7 @@
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>28</v>
       </c>
@@ -1685,45 +2301,59 @@
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
+    <row r="15" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B15" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F15" s="3">
-        <v>0</v>
-      </c>
-      <c r="G15" s="3">
-        <v>2.1150000000000002</v>
-      </c>
-      <c r="H15" s="3">
-        <v>0</v>
-      </c>
-      <c r="I15" s="3">
-        <v>0</v>
-      </c>
-      <c r="J15" s="3">
+      <c r="E15" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="14">
+        <f>1.018+T72/1000</f>
+        <v>1.5580000000000001</v>
+      </c>
+      <c r="G15" s="21">
+        <f>4.133+(T64+T66+T71)/1000</f>
+        <v>4.401583333333333</v>
+      </c>
+      <c r="H15" s="23">
+        <f>1.045+T65/1000</f>
+        <v>1.4869999999999999</v>
+      </c>
+      <c r="I15" s="14">
+        <v>0</v>
+      </c>
+      <c r="J15" s="14">
         <v>0.5</v>
       </c>
-      <c r="K15" s="3">
+      <c r="K15" s="14">
         <v>0.5</v>
       </c>
-      <c r="L15" s="3">
-        <f>0.5+L18</f>
-        <v>1.1879999999999999</v>
+      <c r="L15" s="14">
+        <f>0.5+1.376/2*T65/S65</f>
+        <v>2.5273066666666666</v>
       </c>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="O15">
+        <f>SUM(F15:L15)</f>
+        <v>10.973889999999999</v>
+      </c>
+      <c r="Q15">
+        <v>7.6959999999999997</v>
+      </c>
+      <c r="R15">
+        <f>O15-Q15</f>
+        <v>3.2778899999999993</v>
+      </c>
+    </row>
+    <row r="16" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B16" s="14" t="s">
         <v>32</v>
       </c>
@@ -1739,11 +2369,12 @@
       <c r="F16" s="14">
         <v>0</v>
       </c>
-      <c r="G16" s="14">
-        <v>0.64400000000000002</v>
+      <c r="G16" s="21">
+        <f>1.738+(U64+U66)/1000</f>
+        <v>1.9071666666666667</v>
       </c>
       <c r="H16" s="14">
-        <v>0.14000000000000001</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="I16" s="14">
         <v>0.68400000000000005</v>
@@ -1758,8 +2389,19 @@
         <v>1.5</v>
       </c>
       <c r="N16" s="3"/>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O16">
+        <f>SUM(F16:L16)</f>
+        <v>5.8661666666666665</v>
+      </c>
+      <c r="Q16">
+        <v>5.6970000000000001</v>
+      </c>
+      <c r="R16">
+        <f>O16-Q16</f>
+        <v>0.16916666666666647</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>6</v>
       </c>
@@ -1797,7 +2439,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>35</v>
       </c>
@@ -1817,27 +2459,38 @@
         <v>0</v>
       </c>
       <c r="H18" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18" s="3">
         <v>1</v>
       </c>
       <c r="J18" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L18" s="3">
-        <f>1.376/2</f>
-        <v>0.68799999999999994</v>
+        <f>1.376/2+1</f>
+        <v>1.6879999999999999</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O18">
+        <f>SUM(F18:L18)</f>
+        <v>4.9079999999999995</v>
+      </c>
+      <c r="Q18">
+        <v>4.22</v>
+      </c>
+      <c r="R18">
+        <f>O18-Q18</f>
+        <v>0.68799999999999972</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>37</v>
       </c>
@@ -1874,7 +2527,7 @@
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>39</v>
       </c>
@@ -1910,8 +2563,12 @@
       </c>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O20">
+        <f>SUM(F20:L20)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>41</v>
       </c>
@@ -1948,7 +2605,7 @@
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>43</v>
       </c>
@@ -1985,7 +2642,7 @@
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>45</v>
       </c>
@@ -2022,7 +2679,7 @@
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
         <v>47</v>
       </c>
@@ -2059,7 +2716,7 @@
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25" s="14" t="s">
         <v>49</v>
       </c>
@@ -2073,31 +2730,45 @@
         <v>5</v>
       </c>
       <c r="F25" s="14">
-        <v>0</v>
+        <f>0.275+S65/1000</f>
+        <v>0.42500000000000004</v>
       </c>
       <c r="G25" s="14">
-        <v>0.51300000000000001</v>
+        <f>0.662+(W64+W66+W70+W71)/1000</f>
+        <v>1.03888</v>
       </c>
       <c r="H25" s="14">
-        <v>0</v>
+        <f>W65/1000</f>
+        <v>0.23684210526315788</v>
       </c>
       <c r="I25" s="14">
-        <v>2.6150000000000002</v>
+        <v>2.6160000000000001</v>
       </c>
       <c r="J25" s="14">
-        <v>0.61499999999999999</v>
+        <v>0.61599999999999999</v>
       </c>
       <c r="K25" s="14">
         <v>0</v>
       </c>
       <c r="L25" s="14">
-        <f>L18</f>
-        <v>0.68799999999999994</v>
+        <f>1.376/2*W72/S72</f>
+        <v>1.0319999999999998</v>
       </c>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
-    </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O25">
+        <f>SUM(F25:L25)</f>
+        <v>5.9647221052631583</v>
+      </c>
+      <c r="Q25">
+        <v>4.1689999999999996</v>
+      </c>
+      <c r="R25">
+        <f>O25-Q25</f>
+        <v>1.7957221052631587</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" s="3"/>
       <c r="C26" s="3" t="s">
         <v>63</v>
@@ -2118,7 +2789,7 @@
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>51</v>
       </c>
@@ -2161,8 +2832,12 @@
       </c>
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
-    </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O27">
+        <f t="shared" ref="O27:O31" si="1">SUM(F27:L27)</f>
+        <v>1.125</v>
+      </c>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>53</v>
       </c>
@@ -2176,37 +2851,41 @@
         <v>5</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:L31" si="1">$F34/SUM($F$33:$F$37)*0.9</f>
+        <f t="shared" ref="F28:L31" si="2">$F34/SUM($F$33:$F$37)*0.9</f>
         <v>5.849999999999999E-2</v>
       </c>
       <c r="G28" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.849999999999999E-2</v>
       </c>
       <c r="H28" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.849999999999999E-2</v>
       </c>
       <c r="I28" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.849999999999999E-2</v>
       </c>
       <c r="J28" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.849999999999999E-2</v>
       </c>
       <c r="K28" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.849999999999999E-2</v>
       </c>
       <c r="L28" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.849999999999999E-2</v>
       </c>
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
-    </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O28">
+        <f t="shared" si="1"/>
+        <v>0.40949999999999992</v>
+      </c>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
         <v>55</v>
       </c>
@@ -2220,37 +2899,41 @@
         <v>5</v>
       </c>
       <c r="F29" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.11699999999999998</v>
       </c>
       <c r="G29" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.11699999999999998</v>
       </c>
       <c r="H29" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.11699999999999998</v>
       </c>
       <c r="I29" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.11699999999999998</v>
       </c>
       <c r="J29" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.11699999999999998</v>
       </c>
       <c r="K29" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.11699999999999998</v>
       </c>
       <c r="L29" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.11699999999999998</v>
       </c>
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
-    </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O29">
+        <f t="shared" si="1"/>
+        <v>0.81899999999999984</v>
+      </c>
+    </row>
+    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
         <v>57</v>
       </c>
@@ -2264,37 +2947,41 @@
         <v>5</v>
       </c>
       <c r="F30" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.43457142857142844</v>
       </c>
       <c r="G30" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.43457142857142844</v>
       </c>
       <c r="H30" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.43457142857142844</v>
       </c>
       <c r="I30" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.43457142857142844</v>
       </c>
       <c r="J30" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.43457142857142844</v>
       </c>
       <c r="K30" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.43457142857142844</v>
       </c>
       <c r="L30" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.43457142857142844</v>
       </c>
       <c r="M30" s="3"/>
       <c r="N30" s="3"/>
-    </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O30">
+        <f t="shared" si="1"/>
+        <v>3.0419999999999994</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
         <v>59</v>
       </c>
@@ -2308,37 +2995,41 @@
         <v>5</v>
       </c>
       <c r="F31" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.12921428571428578</v>
       </c>
       <c r="G31" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.12921428571428578</v>
       </c>
       <c r="H31" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.12921428571428578</v>
       </c>
       <c r="I31" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.12921428571428578</v>
       </c>
       <c r="J31" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.12921428571428578</v>
       </c>
       <c r="K31" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.12921428571428578</v>
       </c>
       <c r="L31" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.12921428571428578</v>
       </c>
       <c r="M31" s="3"/>
       <c r="N31" s="3"/>
-    </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O31">
+        <f t="shared" si="1"/>
+        <v>0.9045000000000003</v>
+      </c>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
@@ -2480,12 +3171,12 @@
       <c r="D48" s="5"/>
       <c r="E48" s="6"/>
     </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:35" x14ac:dyDescent="0.25">
       <c r="G49" s="7" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B50" s="8" t="s">
         <v>65</v>
       </c>
@@ -2514,7 +3205,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="s">
         <v>72</v>
       </c>
@@ -2543,7 +3234,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
         <v>72</v>
       </c>
@@ -2572,7 +3263,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B53" s="5" t="s">
         <v>72</v>
       </c>
@@ -2601,7 +3292,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B54" s="5" t="s">
         <v>72</v>
       </c>
@@ -2630,7 +3321,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B55" s="5" t="s">
         <v>72</v>
       </c>
@@ -2659,7 +3350,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B56" s="5" t="s">
         <v>72</v>
       </c>
@@ -2688,7 +3379,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B57" s="5" t="s">
         <v>76</v>
       </c>
@@ -2717,7 +3408,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B58" s="5" t="s">
         <v>76</v>
       </c>
@@ -2747,7 +3438,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B59" s="5" t="s">
         <v>76</v>
       </c>
@@ -2777,7 +3468,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B60" s="5" t="s">
         <v>76</v>
       </c>
@@ -2806,7 +3497,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B61" s="5" t="s">
         <v>76</v>
       </c>
@@ -2835,7 +3526,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B62" s="5" t="s">
         <v>78</v>
       </c>
@@ -2863,8 +3554,20 @@
       <c r="J62" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="T62" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z62" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC62" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF62" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="63" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B63" s="5" t="s">
         <v>78</v>
       </c>
@@ -2892,8 +3595,71 @@
       <c r="J63" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="Q63" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="R63" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="S63" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="T63" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="U63" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="V63" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="W63" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="X63" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y63" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z63" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA63" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB63" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="AC63" t="str">
+        <f t="shared" ref="AC63:AH63" si="3">Z63</f>
+        <v>Solar</v>
+      </c>
+      <c r="AD63" t="str">
+        <f t="shared" si="3"/>
+        <v>Wind</v>
+      </c>
+      <c r="AE63" t="str">
+        <f t="shared" si="3"/>
+        <v>Gas</v>
+      </c>
+      <c r="AF63" t="str">
+        <f t="shared" si="3"/>
+        <v>Solar</v>
+      </c>
+      <c r="AG63" t="str">
+        <f t="shared" si="3"/>
+        <v>Wind</v>
+      </c>
+      <c r="AH63" t="str">
+        <f t="shared" si="3"/>
+        <v>Gas</v>
+      </c>
+      <c r="AI63" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="64" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B64" s="5" t="s">
         <v>78</v>
       </c>
@@ -2921,8 +3687,61 @@
       <c r="J64" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="Q64" t="s">
+        <v>110</v>
+      </c>
+      <c r="R64" s="16">
+        <v>1550.34</v>
+      </c>
+      <c r="S64">
+        <v>128</v>
+      </c>
+      <c r="T64" s="17">
+        <f>AF64/(8.76*Z64)</f>
+        <v>117.33333333333336</v>
+      </c>
+      <c r="U64" s="17">
+        <f>AG64/(8.76*AA64)</f>
+        <v>106.66666666666666</v>
+      </c>
+      <c r="W64">
+        <f>S64</f>
+        <v>128</v>
+      </c>
+      <c r="X64" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="Y64" s="19">
+        <f>S64*X64*8.76</f>
+        <v>560.64</v>
+      </c>
+      <c r="Z64" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="AA64" s="18">
+        <v>0.35</v>
+      </c>
+      <c r="AC64" s="6">
+        <f>(Z64/(Z64+AA64))</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="AD64" s="6">
+        <f>1-AC64</f>
+        <v>0.58333333333333326</v>
+      </c>
+      <c r="AF64">
+        <f>AC64*$Y64*(1+AI64)</f>
+        <v>256.96000000000004</v>
+      </c>
+      <c r="AG64">
+        <f>AD64*$Y64*(1+[1]RMIPPPP!U37)</f>
+        <v>327.03999999999996</v>
+      </c>
+      <c r="AI64" s="18">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="65" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B65" s="5" t="s">
         <v>78</v>
       </c>
@@ -2950,8 +3769,49 @@
       <c r="J65" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="Q65" t="s">
+        <v>111</v>
+      </c>
+      <c r="R65" s="16">
+        <v>1462</v>
+      </c>
+      <c r="S65" s="15">
+        <v>150</v>
+      </c>
+      <c r="T65" s="17">
+        <v>442</v>
+      </c>
+      <c r="W65" s="19">
+        <f>Y65/S122*S121</f>
+        <v>236.84210526315789</v>
+      </c>
+      <c r="X65" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="Y65" s="19">
+        <v>1200</v>
+      </c>
+      <c r="Z65" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="AC65" s="18">
+        <v>1</v>
+      </c>
+      <c r="AF65">
+        <f>AC65*$Y65*(1+AI65)</f>
+        <v>1320</v>
+      </c>
+      <c r="AI65" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="AJ65" t="s">
+        <v>121</v>
+      </c>
+      <c r="AK65" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="66" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B66" s="5" t="s">
         <v>78</v>
       </c>
@@ -2978,10 +3838,341 @@
       </c>
       <c r="J66" s="5">
         <v>5</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>112</v>
+      </c>
+      <c r="R66" s="16">
+        <v>1721.64</v>
+      </c>
+      <c r="S66">
+        <v>75</v>
+      </c>
+      <c r="T66" s="17">
+        <f>AF66/(8.76*Z66)</f>
+        <v>68.75</v>
+      </c>
+      <c r="U66" s="17">
+        <f>AG66/(8.76*AA66)</f>
+        <v>62.499999999999993</v>
+      </c>
+      <c r="W66">
+        <f>S66</f>
+        <v>75</v>
+      </c>
+      <c r="X66" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="Y66" s="19">
+        <f t="shared" ref="Y66:Y71" si="4">S66*X66*8.76</f>
+        <v>328.5</v>
+      </c>
+      <c r="Z66" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="AA66" s="18">
+        <v>0.35</v>
+      </c>
+      <c r="AC66" s="6">
+        <f>AC64</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="AD66" s="6">
+        <f>AD64</f>
+        <v>0.58333333333333326</v>
+      </c>
+      <c r="AF66">
+        <f>AC66*$Y66*(1+AI66)</f>
+        <v>150.5625</v>
+      </c>
+      <c r="AG66">
+        <f>AD66*$Y66*(1+[1]RMIPPPP!U39)</f>
+        <v>191.62499999999997</v>
+      </c>
+      <c r="AI66" s="18">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="67" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="Q67" t="s">
+        <v>113</v>
+      </c>
+      <c r="R67" s="16">
+        <v>1468.87</v>
+      </c>
+      <c r="S67">
+        <v>450</v>
+      </c>
+      <c r="V67">
+        <f>S67</f>
+        <v>450</v>
+      </c>
+      <c r="X67" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="Y67" s="19">
+        <f t="shared" si="4"/>
+        <v>1971</v>
+      </c>
+      <c r="AB67" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="AE67" s="18">
+        <v>1</v>
+      </c>
+      <c r="AI67" s="18">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="68" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="Q68" t="s">
+        <v>114</v>
+      </c>
+      <c r="R68" s="16">
+        <v>1496.03</v>
+      </c>
+      <c r="S68">
+        <v>450</v>
+      </c>
+      <c r="V68">
+        <f>S68</f>
+        <v>450</v>
+      </c>
+      <c r="X68" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="Y68" s="19">
+        <f t="shared" si="4"/>
+        <v>1971</v>
+      </c>
+      <c r="AB68" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="AE68" s="18">
+        <v>1</v>
+      </c>
+      <c r="AI68" s="18">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="69" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="Q69" t="s">
+        <v>115</v>
+      </c>
+      <c r="R69" s="16">
+        <v>1686.48</v>
+      </c>
+      <c r="S69">
+        <v>320</v>
+      </c>
+      <c r="V69">
+        <f>S69</f>
+        <v>320</v>
+      </c>
+      <c r="X69" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="Y69" s="19">
+        <f t="shared" si="4"/>
+        <v>1401.6</v>
+      </c>
+      <c r="AB69" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="AE69" s="18">
+        <v>1</v>
+      </c>
+      <c r="AI69" s="18">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="70" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="Q70" t="s">
+        <v>116</v>
+      </c>
+      <c r="R70" s="16">
+        <v>1885.37</v>
+      </c>
+      <c r="S70">
+        <v>197.76</v>
+      </c>
+      <c r="V70">
+        <f>W70</f>
+        <v>98.88</v>
+      </c>
+      <c r="W70">
+        <f>S70/2</f>
+        <v>98.88</v>
+      </c>
+      <c r="X70" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="Y70" s="19">
+        <f t="shared" si="4"/>
+        <v>866.1887999999999</v>
+      </c>
+      <c r="AB70" s="18">
+        <v>1</v>
+      </c>
+      <c r="AE70" s="18">
+        <v>1</v>
+      </c>
+      <c r="AH70">
+        <f>Y70/2*(1+AI70)+Y70/2</f>
+        <v>909.4982399999999</v>
+      </c>
+      <c r="AI70" s="18">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="71" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="Q71" t="s">
+        <v>117</v>
+      </c>
+      <c r="R71" s="16">
+        <v>1515.97</v>
+      </c>
+      <c r="S71">
+        <v>75</v>
+      </c>
+      <c r="T71" s="17">
+        <f>AF71/(8.76*Z71)</f>
+        <v>82.500000000000014</v>
+      </c>
+      <c r="W71">
+        <f>S71</f>
+        <v>75</v>
+      </c>
+      <c r="X71" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="Y71" s="19">
+        <f t="shared" si="4"/>
+        <v>328.5</v>
+      </c>
+      <c r="Z71" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="AC71" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="AE71" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="AF71">
+        <f>AC71*$Y71*(1+AI71)</f>
+        <v>180.67500000000001</v>
+      </c>
+      <c r="AI71" s="18">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="72" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="Q72" t="s">
+        <v>127</v>
+      </c>
+      <c r="R72" s="16">
+        <v>1884</v>
+      </c>
+      <c r="S72">
+        <v>150</v>
+      </c>
+      <c r="T72">
+        <v>540</v>
+      </c>
+      <c r="W72">
+        <v>225</v>
+      </c>
+      <c r="Y72">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="73" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="Q73" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="T73" s="17">
+        <f>SUM(T64:T72)</f>
+        <v>1250.5833333333335</v>
+      </c>
+      <c r="U73" s="17">
+        <f t="shared" ref="U73:W73" si="5">SUM(U64:U72)</f>
+        <v>169.16666666666666</v>
+      </c>
+      <c r="V73" s="17">
+        <f t="shared" si="5"/>
+        <v>1318.88</v>
+      </c>
+      <c r="W73" s="17">
+        <f t="shared" si="5"/>
+        <v>838.72210526315791</v>
+      </c>
+    </row>
+    <row r="74" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="Q74" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="S74" s="17">
+        <f>W73*0.7+V73</f>
+        <v>1905.9854736842108</v>
+      </c>
+    </row>
+    <row r="75" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="Q75" t="s">
+        <v>129</v>
+      </c>
+      <c r="S75" s="20">
+        <f>S74-SUM(S67:S69)</f>
+        <v>685.98547368421077</v>
+      </c>
+    </row>
+    <row r="77" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="Q77" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="120" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q120" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="S120">
+        <v>540</v>
+      </c>
+      <c r="T120" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="121" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="S121">
+        <v>225</v>
+      </c>
+      <c r="T121" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="U121" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="122" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="S122">
+        <v>1140</v>
+      </c>
+      <c r="T122" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="123" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="S123">
+        <f>S122/S121</f>
+        <v>5.0666666666666664</v>
+      </c>
+      <c r="T123" s="5" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>